<commit_message>
Updated excel description file
</commit_message>
<xml_diff>
--- a/WHEAT_CODES.xlsx
+++ b/WHEAT_CODES.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ONEDRIVE\OneDrive - Pontificia Universidad Javeriana Cali\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\REPO_GITHUB\Trancriptomics_atlas_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54246C05-C5EB-4426-96CB-453220F7081F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EA5DE5-38E1-41AC-B8B6-CA73E0C548FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B76C372A-1E03-4541-958F-C176872B34C2}"/>
+    <workbookView minimized="1" xWindow="3732" yWindow="2412" windowWidth="12540" windowHeight="9948" xr2:uid="{B76C372A-1E03-4541-958F-C176872B34C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$E$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Code</t>
   </si>
@@ -50,13 +51,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>This is an R function that reads count tables generated by Salmon, performs differential expression analysis using the edgeR package, and outputs results and plots. The function takes in several arguments including the name of the folder where the data is stored, the name of the output directory, the significance threshold for differential expression testing, and the number of cores to use for parallelization.
-The code begins by loading required packages including ggplot2, edgeR, tximport, and parallel. It checks if combinefolders is not null and if it is either TRUE or FALSE. The combinefolders argument determines if multiple folders should be processed in one run or if each folder should be processed separately. If combinefolders is TRUE and there is more than one folder, the function will create a new output directory with the name specified in out_name to store the results. If combinefolders is FALSE, the function will create a new output directory with the name of the folder specified in folder_name.
-The function then detects the number of cores available for parallelization using the detectCores function from the parallel package. It checks if the number of cores specified in numCores is less than or equal to the number of cores detected by the function. If numCores is greater than the number of cores detected, the function throws an error.
-Next, the function creates two subdirectories within the output directory named "graphics" and "csv" to store plots and CSV files, respectively. It then reads in the count tables generated by Salmon using the tximport function from the tximport package. It also reads in the metadata file which contains information about the samples such as the experimental conditions and replicates. The function checks if each group has at least two samples and stops if any group has only one sample. The function also checks if a group_vect object has been provided and if it matches the number of samples. If it does not match, the function throws an error. If group_vect is not provided, the function uses the metadata file to define treatments and their levels.
-Finally, the function performs differential expression analysis using the edgeR package, generates diagnostic plots including MDS plots, and outputs the results to CSV files. It also saves the library size and dispersion estimates to files in the output directory.</t>
-  </si>
-  <si>
     <t>gene_intersects.R</t>
   </si>
   <si>
@@ -93,36 +87,126 @@
     <t>Identify pan and core contrasts drought genes</t>
   </si>
   <si>
-    <t>This is a function named "topGO_gen" that performs gene ontology enrichment analysis using topGO R package. The function takes the following arguments:
-ta_go_file: A string indicating the path to the GO annotations file in the text format.
-custom_format: A logical value indicating if the GO annotations file has a custom format. If it is FALSE, the function assumes the annotations file is in the standard format.
-genes_id: A vector containing the gene IDs to be used in the analysis.
-pval: A numeric value indicating the significance threshold (p-value).
-out_dir: A string indicating the path to the output directory.
-output_name: A string indicating the name of the output file.
-background: A vector containing the gene IDs to be used as background for the analysis. If it is NULL, all the genes in the GO annotations file will be used.
-The function first loads the "reducereduntGO_ALL.R" function that reduces redundancy in enrichments using DAG. Then, it loads the required packages, including "data.table", "topGO", "dplyr", "gProfileR", and "GO.db". After that, it reads the GO annotations file using the "fread" function from the data.table package.
-If the annotations file has a custom format, the function subsets the file and changes the column names to "gene_id" and "go". Otherwise, the function changes the column names from "#gene_id" to "gene_id" and subsets the file to keep only the columns "gene_id" and "go". The function then indexes the background genes and subsets them if the "background" argument is provided.
-If the output file does not exist, the function runs gene ontology enrichment analysis using gprofiler2 for the molecular function (MF) domain. The function uses the "reducereduntGOALL" function to reduce redundancy in enrichments and returns the results in a data frame called "all_res1_MF". If there are no significant enriched results, the function returns NULL for "all_res1_MF".
-Next, the function runs gene ontology enrichment analysis using topGO for the biological process (BP) domain. The function first creates a list of gene IDs and their GO terms and formats it to the topGO format. The function then creates a topGO object using the "new" function and runs statistical tests using the "runTest" function. The function gets all the GO terms used and summarizes the results in a data frame called "all_res1". The function returns all the GO terms used to avoid mistakes in the downstream analysis.</t>
-  </si>
-  <si>
-    <t>The function reducereduntGOALL takes four arguments:
-df: a data frame containing the results of a gene ontology (GO) enrichment analysis, where each row represents a GO term and its associated statistics.
+    <t>reducereduntGO_ALL</t>
+  </si>
+  <si>
+    <t>Gene set enrichment analysis refinement</t>
+  </si>
+  <si>
+    <t>folder</t>
+  </si>
+  <si>
+    <t>CODES</t>
+  </si>
+  <si>
+    <t>ADDITIONAL_CODES</t>
+  </si>
+  <si>
+    <t>Arguments</t>
+  </si>
+  <si>
+    <t>Function Body:
+The function first loads several libraries, including ggplot2, edgeR, tximport, and parallel. It then checks the validity of the combinefolders argument to make sure that it is either TRUE or FALSE.
+Next, the function checks if combinefolders is TRUE, and if so, it checks whether there is more than one folder in folder_name. If there is only one folder, the function stops. Otherwise, it prints a message indicating that it is processing multifolders and using out_name to name the output folder.
+The function then detects the number of cores available for parallel processing and checks if numCores exceeds the maximum allowed by the machine. If it does, the function stops and suggests using a coherent number of cores such as four.
+The function creates an output directory folder, out_dir_1, based on whether combinefolders is TRUE. It then defines plot directories and csv directories for contrasts.
+Next, the function reads the salmon files and metadata. It checks if the groups have more than one sample and uses a group_vect object if available. If any group has only one sample, the function stops.
+The function then defines treatments and performs the DE analysis using edgeR. It creates plots if plot_MDS is TRUE, and writes the results to csv files. Finally, the function returns a list of results.</t>
+  </si>
+  <si>
+    <t>Class of code</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Manual steps</t>
+  </si>
+  <si>
+    <t>indir: a character string that represents the path to the directory where the input files are located.
+folder: a character string that represents the name of the folder containing the input files.
+ta_go_file: a character string that represents the path to the file containing the gene ontology annotations.
+custom_format: a logical value indicating whether the gene ontology annotation file is in a custom format (TRUE) or a standard format (FALSE).
+contrasts: a character vector containing the names of the contrasts to be analyzed.
+pval: a numeric value representing the p-value cutoff.</t>
+  </si>
+  <si>
+    <t>combinefolders: a logical value indicating whether to combine several folders into one run. The default value is FALSE.
+out_name: a character string indicating the name of the output folder if combinefolders is TRUE.
+folder_name: a character vector with the name of the folder containing the data.
+pval: a numeric value indicating the p-value threshold for significance.
+out_dir: a character string indicating the output directory.
+met_dir: a character string indicating the directory containing the metadata.
+plot_MDS: a logical value indicating whether to plot multidimensional scaling. The default value is FALSE.
+numCores: a numeric value indicating the number of cores to use.
+group_vect: a character vector indicating the group for each sample.</t>
+  </si>
+  <si>
+    <t>The function first loads several required packages, including data.table, topGO, dplyr, GO.db, and parallel. It then checks whether the input files exist, and stops with an error message if any of them do not exist.
+The gene ontology annotation file (ta_go_file) is read into R using the fread function from the data.table package. If custom_format is FALSE, the function changes the column name #gene_id to gene_id, subsets the columns to gene_id, go, and description, and assigns the resulting data.table to ta_go_file. If custom_format is TRUE, the function assigns the column names "go", "gene_id", and "na" to ta_go_file, subsets the columns to gene_id and go, and assigns the resulting data.table to ta_go_file.
+The function then creates a list of results for each contrast in file. For each contrast, the function reads in the file containing the differentially expressed genes, splits the file into upregulated and downregulated genes, and joins the two lists into genes_stat_list.
+For each direction of differential expression, the function subsets the annotated genes that are in the background set (x_back) and formats them for use in topGO. It then creates a factor indicating whether each gene in x_back is in the list of differentially expressed genes, and creates a topGOdata object using gene_2_GO, which contains the GO term annotations for the genes in x_back.
+The function then runs the runTest function from the topGO package on the topGOdata object, using the "classic" algorithm and "fisher" statistic. It summarizes the results using the GenTable function from the topGO package, and joins the resulting table with a table of p-values to get accurate p-values for each GO term. Finally, the function returns the summarized results for each direction of differential expression for each contrast in file.</t>
+  </si>
+  <si>
+    <t>ta_go_file: the file path to the GO annotation file, which contains gene IDs and GO term annotations.
+custom_format: a logical parameter that indicates whether the input file format is custom or not. If TRUE, the function expects the input file format to be custom, otherwise, it expects the input file format to be GOA.
+genes_id: a vector of gene IDs to be analyzed.
+pval: a p-value threshold for significance.
+out_dir: the output directory path where the results will be saved.
+output_name: a name for the output file.
+background: a vector of gene IDs to be used as the background. If NULL, all unique gene IDs in the ta_go_file will be used.</t>
+  </si>
+  <si>
+    <t>The function begins by loading the reducereduntGO_ALL.R function from a specific file path. Then, it loads the required libraries, including data.table, topGO, dplyr, gProfileR, and GO.db.
+Next, it reads the ta_go_file using fread() from the data.table package. If custom_format is FALSE, the function assumes that the input file is in GOA format and renames the first column to gene_id. It then subsets the data to contain only the gene_id and go columns. If custom_format is TRUE, the function assumes that the input file is in custom format, subsets the data to contain only the gene_id and go columns, and renames them accordingly.
+The function then creates an index to subset the ta_go_file and creates a vector x_back_vect containing only the unique gene_id values in the ta_go_file. If background is not NULL, the function subsets x_back_vect to contain only the gene_id values present in background.
+The function then checks if the output file already exists in the output directory, and if it does, it does not re-run the analysis.
+The function then runs GO enrichment analysis for the molecular function (MF) ontology using gprofiler2::gost() from the gProfileR package. It passes genes_id, "taestivum" as the organism, pval, and unique(x_back_vect$gene_id) as the background to the function. It then uses the reducereduntGOALL() function to reduce redundancy in the results obtained from gprofiler2::gost(). The resulting data frame is stored in all_res1_MF, and if it is empty, NULL is stored instead.
+The function then runs GO enrichment analysis for the biological process (BP) ontology using topGO. It creates a list of gene IDs and their GO terms from the x_back_vect data frame, subsets it to contain only the gene_id values present in genes_id, and converts it to a factor vector. It then creates a topGOdata object containing the ontology, the geneList, the annot function, and the gene_2_GO data frame. It runs topGO::runTest() with the "classic" algorithm and the "fisher" statistic. It then uses topGO::GenTable() to generate a summary of the results, which are stored in all_res1.
+Finally, the function saves the results to a TSV file in the output directory using `write.table</t>
+  </si>
+  <si>
+    <t>This is an R function that takes as input a data frame (df), a GO.ID column name (GO.ID), a FDR column name (FDR_col), and a mode (mode). The function first checks if mode is valid (i.e., "BP", "MF", or "CC") and filters the input data frame by the children terms, evaluating each term. Then, it obtains the children - parent relationships to test them. If there is no available parent - children relationship, it returns the same GO to avoid errors. The function then calculates the FDR values for the children terms and the parental term and selects the GO term with the minimum FDR. Finally, it returns a filtered data frame (df1) with all the output and obtains a filter table. If there are no results available, it returns a warning message.</t>
+  </si>
+  <si>
+    <t>df: a data frame containing the results of a gene ontology (GO) enrichment analysis, where each row represents a GO term and its associated statistics.
 GO.ID: the name of the column in df that contains the GO IDs.
 FDR_col: the name of the column in df that contains the false discovery rate (FDR) values.
-mode: a character string specifying the type of GO terms to filter. It can be one of "BP" (biological process), "MF" (molecular function), or "CC" (cellular component).
-The function first checks if mode is a valid option (BP, MF, or CC). If not, it stops with an error message.
-If df has at least one row, the function proceeds to filter the results by GO terms that have better FDR values among their children terms. The filtering is done separately for each of the three types of GO terms specified by mode.
-For each GO term in df, the function obtains the FDR values of its children terms using the GOCHILDREN object from the GO.db package. If a parent term has no children, its own FDR value is used instead. Then, the function selects the GO term with the lowest FDR value among the parent and children terms as the representative term.
-Finally, the function returns a data frame containing the rows of df that correspond to the filtered GO terms.
-If df is empty, the function returns a warning message and returns the original df unchanged.</t>
-  </si>
-  <si>
-    <t>reducereduntGO_ALL</t>
-  </si>
-  <si>
-    <t>Gene set enrichment analysis refinement</t>
+mode: a character string specifying the type of GO terms to filter. It can be one of "BP" (biological process), "MF" (molecular function), or "CC" (cellular component).</t>
+  </si>
+  <si>
+    <t>PREPARE_FILES_ENRICHER_CONFIDENCE.R</t>
+  </si>
+  <si>
+    <t>Motif enrichment preparation</t>
+  </si>
+  <si>
+    <t>This piece of code  read  the pan and core contrast drought gene lists and write tsv files to run Enricher v.2.4. For this purpose, the code creates four empty lists, two for core and two por pan genes. These four lists represent the combinations of motif unfiltered and filtered by conserved genomic elements in wheat. Finally, it creates a bash file with the folder paths to run Enricher</t>
+  </si>
+  <si>
+    <t>an_dir &lt;- "/scratch/bis_klpoe/chsos/analysis" #analysis dir
+DEG_dir &lt;- "/scratch/bis_klpoe/chsos/analysis/DEG" #DEG dir
+in_dir &lt;- "/scratch/bis_klpoe/chsos/analysis/MOTIF_ENRICHMENT/inputs" #path to save the inputs for  the enrichment analysis
+res_dir &lt;- "/scratch/bis_klpoe/chsos/analysis/MOTIF_ENRICHMENT/results" #path to save the results for  the enrichment analysis
+xx_dir &lt;- "/scratch/bis_klpoe/chsos/analysis/MOTIF_ENRICHMENT" #path to save the bash file to run Enrichr
+CORE_GENES &lt;- as.data.frame(fread(paste0(DEG_dir,"/","LFC_CORE.tsv"),header = T)) #read core genes
+PAN_GENES &lt;- as.data.frame(fread(paste0(DEG_dir,"/","LFC_PAN.tsv"),header = T)) #read pan genes</t>
+  </si>
+  <si>
+    <t>nf-core/rnaseq</t>
+  </si>
+  <si>
+    <t>Run after</t>
+  </si>
+  <si>
+    <t>data_dir &lt;- "/scratch/bis_klpoe/chsos/analysis/GO_DEG" #dir with the TopGO results</t>
+  </si>
+  <si>
+    <t>This piece of code joins the results of gene set enrichment analysis  found by TopGO.R function. The code compiles all the subfolder found in the GSEA for up and downregulated genes and save it in a tsv file. Further, the code creates the inputs for upset plots to explore visually the amount of GO terms intersected across contrasts. Finally, it extracts the top ten of enriched GO terms per contrast and fill out using the information saved in the DEG dir to create a heatmap summarizing the behavior of upregulated and downregulated biological processes found per contrast.</t>
+  </si>
+  <si>
+    <t>Important files created</t>
   </si>
 </sst>
 </file>
@@ -480,105 +564,228 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68DD42A0-FB82-4441-8C8D-04A848DF6B06}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="36.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.109375" style="1"/>
-    <col min="3" max="3" width="91.6640625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="36.109375" style="1"/>
+    <col min="1" max="1" width="44.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="112.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.109375" style="2"/>
+    <col min="8" max="16384" width="36.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="403.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="187.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C8" xr:uid="{68DD42A0-FB82-4441-8C8D-04A848DF6B06}"/>
+  <autoFilter ref="A1:E8" xr:uid="{68DD42A0-FB82-4441-8C8D-04A848DF6B06}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F0A70A-2818-4DBB-9A2D-940D0011ABDD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>